<commit_message>
updated networking/facilities ongoing costs
</commit_message>
<xml_diff>
--- a/cloud_cost_comparison.xlsx
+++ b/cloud_cost_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsettlag/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFDE584-8596-4A49-BB01-886EABFF14F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA36A08-80D6-984C-8707-9CC7AA477BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="1780" windowWidth="29260" windowHeight="19120" activeTab="7" xr2:uid="{19882325-6CB8-BD46-ADED-9ABB001A07F8}"/>
+    <workbookView xWindow="4340" yWindow="1780" windowWidth="29260" windowHeight="19120" xr2:uid="{19882325-6CB8-BD46-ADED-9ABB001A07F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost comparison" sheetId="1" r:id="rId1"/>
@@ -312,9 +312,6 @@
     <t>k80???</t>
   </si>
   <si>
-    <t>Networking (0.5) and facilities (0.5) on-going cost (1 FTE)</t>
-  </si>
-  <si>
     <t>NOTE 2: thread counts and node unit costs based on Cray quote (308 nodes rounded up to $10.6k/node inclusive of support nodes, service contract and Bright for 5 years)</t>
   </si>
   <si>
@@ -484,6 +481,9 @@
   </si>
   <si>
     <t>Total VM for class</t>
+  </si>
+  <si>
+    <t>Networking and facilities on-going cost (1 FTE + $85k/year)</t>
   </si>
 </sst>
 </file>
@@ -499,8 +499,8 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00000_);[Red]\(&quot;$&quot;#,##0.00000\)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1317,15 +1317,15 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1355,11 +1355,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="179" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="4" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1378,30 +1378,21 @@
     <xf numFmtId="165" fontId="4" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="3" fillId="12" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="12" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="3" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1421,13 +1412,22 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1747,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC89DB2-783B-4744-8087-B4E01E2C33B2}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1768,174 +1768,174 @@
   <sheetData>
     <row r="1" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E1" s="61"/>
       <c r="F1" s="61"/>
       <c r="J1" s="61"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D2" s="162" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="165" t="s">
+      <c r="D2" s="187" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="164" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="165" t="s">
-        <v>136</v>
-      </c>
-      <c r="I2" s="165" t="s">
-        <v>141</v>
-      </c>
-      <c r="J2" s="170"/>
+      <c r="H2" s="164" t="s">
+        <v>135</v>
+      </c>
+      <c r="I2" s="164" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="168"/>
     </row>
     <row r="3" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="13"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="173" t="s">
+      <c r="D3" s="187"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="173"/>
-      <c r="I3" s="173"/>
-      <c r="J3" s="171"/>
+      <c r="H3" s="185"/>
+      <c r="I3" s="185"/>
+      <c r="J3" s="169"/>
     </row>
     <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="174" t="s">
+      <c r="B4" s="171" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="175" t="s">
+      <c r="C4" s="172" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="176">
+      <c r="D4" s="173">
         <f>'Actual used CPU'!F6</f>
         <v>1426091915.3160923</v>
       </c>
       <c r="E4" s="62"/>
-      <c r="F4" s="174" t="s">
+      <c r="F4" s="171" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="179">
+      <c r="G4" s="176">
         <f>D4/12*'ON-PREM'!F19+'ON-PREM'!F30*5/12*(D4/12)/20000</f>
-        <v>242982.69995964546</v>
-      </c>
-      <c r="H4" s="179">
+        <v>246957.20876686828</v>
+      </c>
+      <c r="H4" s="176">
         <f>D4/12*'AWS compute'!I15</f>
         <v>5773691.5738144582</v>
       </c>
-      <c r="I4" s="180">
+      <c r="I4" s="177">
         <f>H4*0.36</f>
         <v>2078528.9665732048</v>
       </c>
-      <c r="J4" s="166"/>
+      <c r="J4" s="165"/>
       <c r="K4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="174" t="s">
+      <c r="B5" s="171" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="175" t="s">
+      <c r="C5" s="172" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="176">
+      <c r="D5" s="173">
         <f>'Actual used CPU'!F7</f>
         <v>10133724.425287358</v>
       </c>
       <c r="E5" s="62"/>
-      <c r="F5" s="174" t="s">
+      <c r="F5" s="171" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="179">
+      <c r="G5" s="176">
         <f>D5/12*'ON-PREM'!F19+'Cost comparison'!G32/12*500/1024*(D5/12)/20000</f>
-        <v>1326.304978198187</v>
-      </c>
-      <c r="H5" s="179">
+        <v>1354.5476016544362</v>
+      </c>
+      <c r="H5" s="176">
         <f>D5/12*'AWS web'!I17</f>
         <v>127182.1824301884</v>
       </c>
-      <c r="I5" s="180">
+      <c r="I5" s="177">
         <f t="shared" ref="I5:I7" si="0">H5*0.36</f>
         <v>45785.585674867827</v>
       </c>
-      <c r="J5" s="166"/>
+      <c r="J5" s="165"/>
       <c r="K5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="174" t="s">
+      <c r="B6" s="171" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="175" t="s">
+      <c r="C6" s="172" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="176">
+      <c r="D6" s="173">
         <f>'Actual used CPU'!F8</f>
         <v>10416655.925925925</v>
       </c>
       <c r="E6" s="62"/>
-      <c r="F6" s="174" t="s">
+      <c r="F6" s="171" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="179">
+      <c r="G6" s="176">
         <f>D6/12*'ON-PREM'!F19+'ON-PREM'!F30/12*5*(D6/12)/20000</f>
-        <v>1774.8275228606931</v>
-      </c>
-      <c r="H6" s="179">
+        <v>1803.8586745520802</v>
+      </c>
+      <c r="H6" s="176">
         <f>D6/12*'AWS HM'!I15</f>
         <v>60752.97555131172</v>
       </c>
-      <c r="I6" s="180">
+      <c r="I6" s="177">
         <f t="shared" si="0"/>
         <v>21871.071198472218</v>
       </c>
-      <c r="J6" s="166"/>
+      <c r="J6" s="165"/>
       <c r="K6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="174" t="s">
+      <c r="B7" s="171" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="175" t="s">
+      <c r="C7" s="172" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="176">
+      <c r="D7" s="173">
         <f>'Actual used CPU'!F9</f>
         <v>1618684.2031848659</v>
       </c>
       <c r="E7" s="62"/>
-      <c r="F7" s="174" t="s">
+      <c r="F7" s="171" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="179">
+      <c r="G7" s="176">
         <f>D7/12*'ON-PREM'!F19*(12)*(30/10.6)+'ON-PREM'!F30*5/12*D7/12/20000</f>
-        <v>7258.9810799363804</v>
-      </c>
-      <c r="H7" s="179">
+        <v>7412.1937601030313</v>
+      </c>
+      <c r="H7" s="176">
         <f>D7/12*'AWS GPU'!I15</f>
         <v>462943.68211087165</v>
       </c>
-      <c r="I7" s="180">
+      <c r="I7" s="177">
         <f t="shared" si="0"/>
         <v>166659.72555991379</v>
       </c>
-      <c r="J7" s="166"/>
+      <c r="J7" s="165"/>
       <c r="K7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="17"/>
       <c r="G8" s="16">
         <f>SUM(G4:G7)</f>
-        <v>253342.81354064072</v>
+        <v>257527.80880317782</v>
       </c>
       <c r="H8" s="16">
         <f>SUM(H4:H7)</f>
@@ -1945,7 +1945,7 @@
         <f>SUM(I4:I7)</f>
         <v>2312845.3490064591</v>
       </c>
-      <c r="J8" s="172"/>
+      <c r="J8" s="170"/>
       <c r="K8" t="s">
         <v>70</v>
       </c>
@@ -1956,32 +1956,32 @@
     <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="61"/>
       <c r="B10" s="18"/>
-      <c r="G10" s="173" t="s">
+      <c r="G10" s="185" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="173"/>
-      <c r="I10" s="173"/>
+      <c r="H10" s="185"/>
+      <c r="I10" s="185"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="D11" s="61"/>
-      <c r="F11" s="174" t="s">
+      <c r="F11" s="171" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="180">
+      <c r="G11" s="177">
         <f>G4*12</f>
-        <v>2915792.3995157452</v>
-      </c>
-      <c r="H11" s="180">
+        <v>2963486.5052024191</v>
+      </c>
+      <c r="H11" s="177">
         <f t="shared" ref="H11:I11" si="1">H4*12</f>
         <v>69284298.885773495</v>
       </c>
-      <c r="I11" s="180">
+      <c r="I11" s="177">
         <f t="shared" si="1"/>
         <v>24942347.598878458</v>
       </c>
-      <c r="J11" s="166"/>
+      <c r="J11" s="165"/>
     </row>
     <row r="12" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="19" t="s">
@@ -1990,22 +1990,22 @@
       <c r="D12" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="174" t="s">
+      <c r="F12" s="171" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="180">
+      <c r="G12" s="177">
         <f t="shared" ref="G12:I14" si="2">G5*12</f>
-        <v>15915.659738378243</v>
-      </c>
-      <c r="H12" s="180">
+        <v>16254.571219853235</v>
+      </c>
+      <c r="H12" s="177">
         <f t="shared" si="2"/>
         <v>1526186.1891622609</v>
       </c>
-      <c r="I12" s="180">
+      <c r="I12" s="177">
         <f t="shared" si="2"/>
         <v>549427.02809841395</v>
       </c>
-      <c r="J12" s="166"/>
+      <c r="J12" s="165"/>
     </row>
     <row r="13" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
@@ -2013,77 +2013,77 @@
       </c>
       <c r="C13" s="14">
         <f>'ON-PREM'!H9</f>
-        <v>308069.44444440695</v>
+        <v>314319.44444440695</v>
       </c>
       <c r="D13" s="15">
         <f>C13*12</f>
-        <v>3696833.3333328832</v>
-      </c>
-      <c r="E13" s="166"/>
-      <c r="F13" s="174" t="s">
+        <v>3771833.3333328832</v>
+      </c>
+      <c r="E13" s="165"/>
+      <c r="F13" s="171" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="180">
+      <c r="G13" s="177">
         <f t="shared" si="2"/>
-        <v>21297.930274328319</v>
-      </c>
-      <c r="H13" s="180">
+        <v>21646.30409462496</v>
+      </c>
+      <c r="H13" s="177">
         <f t="shared" si="2"/>
         <v>729035.70661574067</v>
       </c>
-      <c r="I13" s="180">
+      <c r="I13" s="177">
         <f t="shared" si="2"/>
         <v>262452.85438166664</v>
       </c>
-      <c r="J13" s="166"/>
+      <c r="J13" s="165"/>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C14" s="27">
         <f>G8</f>
-        <v>253342.81354064072</v>
+        <v>257527.80880317782</v>
       </c>
       <c r="D14" s="28">
         <f t="shared" ref="D14" si="3">C14*12</f>
-        <v>3040113.7624876886</v>
-      </c>
-      <c r="E14" s="166"/>
-      <c r="F14" s="174" t="s">
+        <v>3090333.7056381339</v>
+      </c>
+      <c r="E14" s="165"/>
+      <c r="F14" s="171" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="180">
+      <c r="G14" s="177">
         <f t="shared" si="2"/>
-        <v>87107.772959236565</v>
-      </c>
-      <c r="H14" s="180">
+        <v>88946.325121236383</v>
+      </c>
+      <c r="H14" s="177">
         <f t="shared" si="2"/>
         <v>5555324.1853304598</v>
       </c>
-      <c r="I14" s="180">
+      <c r="I14" s="177">
         <f t="shared" si="2"/>
         <v>1999916.7067189654</v>
       </c>
-      <c r="J14" s="166"/>
+      <c r="J14" s="165"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="18">
         <f>C14/C13</f>
-        <v>0.82235618659791498</v>
+        <v>0.81931873243917697</v>
       </c>
       <c r="D15" s="18">
         <f>D14/D13</f>
-        <v>0.82235618659791498</v>
-      </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
+        <v>0.81931873243917708</v>
+      </c>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
       <c r="G15" s="16">
         <f>SUM(G11:G14)</f>
-        <v>3040113.7624876881</v>
+        <v>3090333.7056381339</v>
       </c>
       <c r="H15" s="16">
         <f t="shared" ref="H15:I15" si="4">SUM(H11:H14)</f>
@@ -2093,7 +2093,7 @@
         <f t="shared" si="4"/>
         <v>27754144.188077506</v>
       </c>
-      <c r="J15" s="172"/>
+      <c r="J15" s="170"/>
       <c r="K15" t="s">
         <v>71</v>
       </c>
@@ -2105,98 +2105,97 @@
     <row r="17" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="63"/>
       <c r="B17" s="64"/>
-      <c r="G17" s="173" t="s">
+      <c r="G17" s="185" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
+      <c r="H17" s="185"/>
+      <c r="I17" s="185"/>
     </row>
     <row r="18" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="65"/>
       <c r="B18" s="66"/>
-      <c r="F18" s="174" t="s">
+      <c r="F18" s="171" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="180">
+      <c r="G18" s="177">
         <f>G11*5</f>
-        <v>14578961.997578725</v>
-      </c>
-      <c r="H18" s="180">
+        <v>14817432.526012097</v>
+      </c>
+      <c r="H18" s="177">
         <f t="shared" ref="H18:I18" si="5">H11*5</f>
         <v>346421494.42886746</v>
       </c>
-      <c r="I18" s="180">
+      <c r="I18" s="177">
         <f t="shared" si="5"/>
         <v>124711737.99439229</v>
       </c>
-      <c r="J18" s="166"/>
+      <c r="J18" s="165"/>
     </row>
     <row r="19" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="171" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="180">
+      <c r="G19" s="177">
         <f t="shared" ref="G19:I21" si="6">G12*5</f>
-        <v>79578.298691891221</v>
-      </c>
-      <c r="H19" s="180">
+        <v>81272.856099266181</v>
+      </c>
+      <c r="H19" s="177">
         <f t="shared" si="6"/>
         <v>7630930.9458113043</v>
       </c>
-      <c r="I19" s="180">
+      <c r="I19" s="177">
         <f t="shared" si="6"/>
         <v>2747135.1404920695</v>
       </c>
-      <c r="J19" s="166"/>
+      <c r="J19" s="165"/>
     </row>
     <row r="20" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="171" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="180">
+      <c r="G20" s="177">
         <f t="shared" si="6"/>
-        <v>106489.65137164159</v>
-      </c>
-      <c r="H20" s="180">
+        <v>108231.52047312481</v>
+      </c>
+      <c r="H20" s="177">
         <f t="shared" si="6"/>
         <v>3645178.5330787031</v>
       </c>
-      <c r="I20" s="180">
+      <c r="I20" s="177">
         <f t="shared" si="6"/>
         <v>1312264.2719083331</v>
       </c>
-      <c r="J20" s="166"/>
+      <c r="J20" s="165"/>
     </row>
     <row r="21" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="61"/>
       <c r="C21" s="61"/>
       <c r="D21" s="61"/>
-      <c r="F21" s="174" t="s">
+      <c r="F21" s="171" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="180">
+      <c r="G21" s="177">
         <f t="shared" si="6"/>
-        <v>435538.86479618284</v>
-      </c>
-      <c r="H21" s="180">
+        <v>444731.62560618191</v>
+      </c>
+      <c r="H21" s="177">
         <f t="shared" si="6"/>
         <v>27776620.926652297</v>
       </c>
-      <c r="I21" s="180">
+      <c r="I21" s="177">
         <f t="shared" si="6"/>
         <v>9999583.5335948281</v>
       </c>
-      <c r="J21" s="166"/>
+      <c r="J21" s="165"/>
       <c r="K21" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C22"/>
-      <c r="D22"/>
+      <c r="B22"/>
       <c r="G22" s="16">
         <f>SUM(G18:G21)</f>
-        <v>15200568.81243844</v>
+        <v>15451668.528190669</v>
       </c>
       <c r="H22" s="16">
         <f t="shared" ref="H22" si="7">SUM(H18:H21)</f>
@@ -2206,151 +2205,154 @@
         <f t="shared" ref="I22" si="8">SUM(I18:I21)</f>
         <v>138770720.94038752</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="170"/>
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" s="61" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="19"/>
+    <row r="23" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C23"/>
+      <c r="D23"/>
       <c r="L23"/>
       <c r="M23"/>
     </row>
     <row r="24" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="182" t="s">
-        <v>138</v>
-      </c>
-      <c r="B24" s="184">
-        <f>('ON-PREM'!F16+'ON-PREM'!F29)/SUM('Cost comparison'!D4:D6)</f>
-        <v>2.5554577965851695E-3</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="169"/>
-      <c r="E24" s="169"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="19"/>
       <c r="G24" s="61"/>
       <c r="H24" s="61"/>
       <c r="I24" s="61"/>
     </row>
     <row r="25" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="182" t="s">
-        <v>139</v>
-      </c>
-      <c r="B25" s="184">
-        <f>B24/C15</f>
-        <v>3.1074829109720577E-3</v>
+      <c r="A25" s="179" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="181">
+        <f>('ON-PREM'!F16+'ON-PREM'!F29)/SUM('Cost comparison'!D4:D6)</f>
+        <v>2.6073019879409905E-3</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="169"/>
-      <c r="E25" s="169"/>
+      <c r="D25" s="188"/>
+      <c r="E25" s="188"/>
     </row>
     <row r="26" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="183" t="s">
+      <c r="A26" s="179" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="181">
+        <f>B25/C15</f>
+        <v>3.1822804541266196E-3</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="188"/>
+      <c r="E26" s="188"/>
+    </row>
+    <row r="27" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="185">
+      <c r="B27" s="182">
         <f>'AWS web'!C19</f>
         <v>0.15060466666666666</v>
       </c>
-      <c r="C26" s="186">
-        <f>B26*0.36</f>
+      <c r="C27" s="183">
+        <f>B27*0.36</f>
         <v>5.4217679999999997E-2</v>
       </c>
-      <c r="D26" s="187">
-        <f>C26/B25</f>
-        <v>17.447458780405668</v>
-      </c>
-      <c r="E26" s="187"/>
-    </row>
-    <row r="27" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="183" t="s">
+      <c r="D27" s="189">
+        <f>C27/B26</f>
+        <v>17.037367001922558</v>
+      </c>
+      <c r="E27" s="189"/>
+    </row>
+    <row r="28" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="180" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="185">
+      <c r="B28" s="182">
         <f>'AWS compute'!C17</f>
         <v>4.8583333333333339E-2</v>
       </c>
-      <c r="C27" s="186">
-        <f t="shared" ref="C27:C29" si="9">B27*0.36</f>
+      <c r="C28" s="183">
+        <f t="shared" ref="C28:C30" si="9">B28*0.36</f>
         <v>1.7490000000000002E-2</v>
       </c>
-      <c r="D27" s="187">
-        <f>C27/B25</f>
-        <v>5.6283495359686215</v>
-      </c>
-      <c r="E27" s="187"/>
-    </row>
-    <row r="28" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="183" t="s">
+      <c r="D28" s="189">
+        <f>C28/B26</f>
+        <v>5.4960586447746484</v>
+      </c>
+      <c r="E28" s="189"/>
+    </row>
+    <row r="29" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="180" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="185">
+      <c r="B29" s="182">
         <f>'AWS HM'!C17</f>
         <v>6.9987499999999994E-2</v>
       </c>
-      <c r="C28" s="186">
+      <c r="C29" s="183">
         <f t="shared" si="9"/>
         <v>2.5195499999999996E-2</v>
       </c>
-      <c r="D28" s="187">
-        <f>C28/B25</f>
-        <v>8.1080091900227185</v>
-      </c>
-      <c r="E28" s="187"/>
-    </row>
-    <row r="29" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="183" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="185">
+      <c r="D29" s="189">
+        <f>C29/B26</f>
+        <v>7.9174354250668735</v>
+      </c>
+      <c r="E29" s="189"/>
+      <c r="F29" s="178"/>
+    </row>
+    <row r="30" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="180" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="182">
         <f>'AWS GPU'!C17</f>
         <v>3.4319999999999999</v>
       </c>
-      <c r="C29" s="186">
+      <c r="C30" s="183">
         <f t="shared" si="9"/>
         <v>1.23552</v>
       </c>
-      <c r="D29" s="188">
-        <f>C29/(B25)*(30/10.6)</f>
-        <v>1125.2691703097107</v>
-      </c>
-      <c r="E29" s="188"/>
-      <c r="F29" s="181"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F30" s="181"/>
+      <c r="D30" s="186">
+        <f>C30/(B26)*(30/10.6)</f>
+        <v>1098.820411144693</v>
+      </c>
+      <c r="E30" s="186"/>
+      <c r="F30" s="178"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F31" s="177"/>
+      <c r="F31" s="174"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F32" s="177"/>
+      <c r="F32" s="174"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F33" s="177"/>
+      <c r="F33" s="174"/>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="178"/>
+      <c r="F34" s="175"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2361,7 +2363,7 @@
   <dimension ref="B1:N40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2382,7 +2384,7 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
@@ -2405,7 +2407,7 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2428,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -2470,7 +2472,7 @@
     </row>
     <row r="9" spans="2:14" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="140" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="141">
         <f>4+11/12</f>
@@ -2488,7 +2490,7 @@
       </c>
       <c r="H9" s="10">
         <f>G22/12</f>
-        <v>308069.44444440695</v>
+        <v>314319.44444440695</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>74</v>
@@ -2496,7 +2498,7 @@
     </row>
     <row r="10" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="144" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="145">
         <f>B6</f>
@@ -2514,12 +2516,12 @@
       </c>
       <c r="H10" s="4">
         <f>((F17*1000)+F29)/12</f>
-        <v>308069.44444440695</v>
+        <v>314319.44444440695</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="144" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="147">
         <v>2.5</v>
@@ -2555,25 +2557,25 @@
     </row>
     <row r="13" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="144" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="C13" s="147">
         <v>1</v>
       </c>
       <c r="D13" s="146">
-        <v>135000</v>
+        <v>210000</v>
       </c>
       <c r="E13" s="39">
         <v>1</v>
       </c>
       <c r="F13" s="95">
         <f t="shared" si="0"/>
-        <v>135000</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="144" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="147">
         <v>0</v>
@@ -2615,7 +2617,7 @@
       </c>
       <c r="F16" s="154">
         <f>SUM(F9:F15)</f>
-        <v>3522083.3333333335</v>
+        <v>3597083.3333333335</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -2624,7 +2626,7 @@
       </c>
       <c r="F17" s="95">
         <f>SUM(F9:F15)/B6</f>
-        <v>3522.0833333333335</v>
+        <v>3597.0833333333335</v>
       </c>
       <c r="H17" s="4"/>
     </row>
@@ -2634,7 +2636,7 @@
       </c>
       <c r="F18" s="95">
         <f>F17/E6</f>
-        <v>13.758138020833334</v>
+        <v>14.051106770833334</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -2643,7 +2645,7 @@
       </c>
       <c r="F19" s="155">
         <f>F18/365/24</f>
-        <v>1.5705637010083714E-3</v>
+        <v>1.6040076222412483E-3</v>
       </c>
       <c r="H19" s="4"/>
     </row>
@@ -2654,7 +2656,7 @@
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G22" s="23">
         <f>F16+F29</f>
-        <v>3696833.3333328837</v>
+        <v>3771833.3333328837</v>
       </c>
       <c r="H22" s="24" t="s">
         <v>81</v>
@@ -2671,7 +2673,7 @@
       <c r="F23" s="20"/>
       <c r="G23" s="10">
         <f>G22/12</f>
-        <v>308069.44444440695</v>
+        <v>314319.44444440695</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>74</v>
@@ -2730,7 +2732,7 @@
         <v>13500</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -2763,7 +2765,7 @@
     </row>
     <row r="30" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E30" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" s="58">
         <f>F29/7.5/1024</f>
@@ -2783,7 +2785,7 @@
     <row r="32" spans="2:9" ht="20" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -2794,7 +2796,7 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2816,7 +2818,7 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -2827,7 +2829,7 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
@@ -2860,7 +2862,7 @@
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -2891,43 +2893,43 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C4" s="69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D4" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="69" t="s">
-        <v>110</v>
-      </c>
       <c r="F4" s="69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F5" s="70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="159">
         <v>190</v>
@@ -2951,7 +2953,7 @@
     </row>
     <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="159"/>
       <c r="C7" s="160">
@@ -2960,17 +2962,17 @@
       </c>
       <c r="D7" s="159"/>
       <c r="E7" s="161">
-        <f t="shared" ref="E7:E9" si="0">C7*(12/4)*(1000/232)*(128/32)</f>
+        <f t="shared" ref="E7" si="0">C7*(12/4)*(1000/232)*(128/32)</f>
         <v>5066862.2126436792</v>
       </c>
       <c r="F7" s="161">
-        <f t="shared" ref="F7:F9" si="1">E7*2</f>
+        <f t="shared" ref="F7:F8" si="1">E7*2</f>
         <v>10133724.425287358</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="159">
         <v>2</v>
@@ -2994,7 +2996,7 @@
     </row>
     <row r="9" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="159">
         <v>40</v>
@@ -3018,7 +3020,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -3030,12 +3032,12 @@
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" s="68"/>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" s="68"/>
-      <c r="E19" s="163">
+      <c r="E19" s="162">
         <f>F9/24</f>
         <v>67445.175132702745</v>
       </c>
@@ -3084,7 +3086,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="79" t="s">
         <v>45</v>
@@ -3102,7 +3104,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3229,7 +3231,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -3250,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -3270,7 +3272,7 @@
     </row>
     <row r="13" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="87"/>
       <c r="D13" s="88"/>
@@ -3325,7 +3327,7 @@
       <c r="F16" s="88"/>
       <c r="G16" s="88"/>
       <c r="H16" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I16" s="156">
         <f>I15/C3</f>
@@ -3340,14 +3342,14 @@
       <c r="F17" s="88"/>
       <c r="G17" s="88"/>
       <c r="H17" s="93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I17" s="106">
         <f>I16/2</f>
         <v>0.15060466666666666</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="20" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3515,7 +3517,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="79" t="s">
         <v>45</v>
@@ -3533,7 +3535,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -3605,7 +3607,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -3626,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -3701,7 +3703,7 @@
       <c r="F14" s="88"/>
       <c r="G14" s="88"/>
       <c r="H14" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I14" s="157">
         <f>I13/C3</f>
@@ -3716,7 +3718,7 @@
       <c r="F15" s="88"/>
       <c r="G15" s="88"/>
       <c r="H15" s="93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I15" s="106">
         <f>I14/F6</f>
@@ -3921,7 +3923,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="79" t="s">
         <v>45</v>
@@ -3939,7 +3941,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -4011,7 +4013,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -4032,7 +4034,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -4107,7 +4109,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I14" s="156">
         <f>I13/C3</f>
@@ -4122,7 +4124,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I15" s="106">
         <f>I14/F6</f>
@@ -4330,7 +4332,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="79" t="s">
         <v>45</v>
@@ -4339,16 +4341,16 @@
         <v>21</v>
       </c>
       <c r="F5" s="79" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" s="79" t="s">
         <v>35</v>
       </c>
       <c r="H5" s="80" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I5" s="109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -4363,7 +4365,7 @@
         <f>C6*C3/12</f>
         <v>1666.6666666666667</v>
       </c>
-      <c r="E6" s="164">
+      <c r="E6" s="163">
         <v>3.06</v>
       </c>
       <c r="F6" s="134">
@@ -4420,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -4441,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -4516,7 +4518,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I14" s="156">
         <f>I13/C3</f>
@@ -4532,7 +4534,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I15" s="105">
         <f>I14/F6</f>
@@ -4553,7 +4555,7 @@
     </row>
     <row r="17" spans="2:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" s="138">
         <f>I14</f>
@@ -4685,7 +4687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB88280-D265-3244-8D3C-7D721287C2D0}">
   <dimension ref="B1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -4698,7 +4700,7 @@
   <sheetData>
     <row r="1" spans="2:11" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -4720,14 +4722,14 @@
     </row>
     <row r="3" spans="2:11" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1">
         <f>12*4*5</f>
         <v>240</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4750,7 +4752,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="79" t="s">
         <v>45</v>
@@ -4768,7 +4770,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4837,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -4858,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -4869,7 +4871,7 @@
       <c r="F10" s="86"/>
       <c r="G10" s="86"/>
       <c r="H10" s="75" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I10" s="100">
         <f>SUM(I6:I9)</f>
@@ -4878,7 +4880,7 @@
     </row>
     <row r="11" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="87"/>
       <c r="D11" s="88"/>
@@ -4901,7 +4903,7 @@
       <c r="F12" s="88"/>
       <c r="G12" s="88"/>
       <c r="H12" s="88" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I12" s="100">
         <f>I11+I10</f>
@@ -4918,7 +4920,7 @@
       <c r="F13" s="88"/>
       <c r="G13" s="88"/>
       <c r="H13" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I13" s="156">
         <f>I12/C3</f>
@@ -4933,7 +4935,7 @@
       <c r="F14" s="88"/>
       <c r="G14" s="88"/>
       <c r="H14" s="93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I14" s="106">
         <f>I13/F6</f>
@@ -4972,7 +4974,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="I17" s="189">
+      <c r="I17" s="184">
         <f>I14*0.36</f>
         <v>4.1349000000000004E-3</v>
       </c>

</xml_diff>

<commit_message>
fixed GPU and tiny cost errors in sheet
GPU cost didn't reflect proper scaling from CPU -- 2 GPU vs 128 cores and $30k/node vs $10.6k
</commit_message>
<xml_diff>
--- a/cloud_cost_comparison.xlsx
+++ b/cloud_cost_comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsettlag/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsettlag/Projects/Papers/Cloud_paper_cascades_utilization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA36A08-80D6-984C-8707-9CC7AA477BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC63F669-BED6-E949-83E5-384462E3DDD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="1780" windowWidth="29260" windowHeight="19120" xr2:uid="{19882325-6CB8-BD46-ADED-9ABB001A07F8}"/>
+    <workbookView xWindow="2760" yWindow="1020" windowWidth="25760" windowHeight="18220" xr2:uid="{19882325-6CB8-BD46-ADED-9ABB001A07F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost comparison" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="150">
   <si>
     <t>Number of nodes</t>
   </si>
@@ -484,13 +484,19 @@
   </si>
   <si>
     <t>Networking and facilities on-going cost (1 FTE + $85k/year)</t>
+  </si>
+  <si>
+    <t>this reflects a 2 volta node cost 30k vs 10.6k for a CPU only</t>
+  </si>
+  <si>
+    <t>this also includes backing out the cores/node and dividing by 2 GPU/node</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -501,6 +507,7 @@
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="173" formatCode="0.00000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1187,7 +1194,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1411,7 +1418,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1427,6 +1433,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1747,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC89DB2-783B-4744-8087-B4E01E2C33B2}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1775,7 +1785,7 @@
       <c r="J1" s="61"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D2" s="187" t="s">
+      <c r="D2" s="186" t="s">
         <v>132</v>
       </c>
       <c r="E2" s="167"/>
@@ -1793,14 +1803,14 @@
     </row>
     <row r="3" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="13"/>
-      <c r="D3" s="187"/>
+      <c r="D3" s="186"/>
       <c r="E3" s="167"/>
       <c r="F3" s="167"/>
-      <c r="G3" s="185" t="s">
+      <c r="G3" s="184" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
       <c r="J3" s="169"/>
     </row>
     <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1856,11 +1866,11 @@
       </c>
       <c r="H5" s="176">
         <f>D5/12*'AWS web'!I17</f>
-        <v>127182.1824301884</v>
+        <v>10598.5152025157</v>
       </c>
       <c r="I5" s="177">
         <f t="shared" ref="I5:I7" si="0">H5*0.36</f>
-        <v>45785.585674867827</v>
+        <v>3815.4654729056519</v>
       </c>
       <c r="J5" s="165"/>
       <c r="K5" t="s">
@@ -1939,11 +1949,11 @@
       </c>
       <c r="H8" s="16">
         <f>SUM(H4:H7)</f>
-        <v>6424570.4139068294</v>
+        <v>6307986.746679157</v>
       </c>
       <c r="I8" s="16">
         <f>SUM(I4:I7)</f>
-        <v>2312845.3490064591</v>
+        <v>2270875.2288044961</v>
       </c>
       <c r="J8" s="170"/>
       <c r="K8" t="s">
@@ -1956,11 +1966,11 @@
     <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="61"/>
       <c r="B10" s="18"/>
-      <c r="G10" s="185" t="s">
+      <c r="G10" s="184" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="185"/>
-      <c r="I10" s="185"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1999,11 +2009,11 @@
       </c>
       <c r="H12" s="177">
         <f t="shared" si="2"/>
-        <v>1526186.1891622609</v>
+        <v>127182.1824301884</v>
       </c>
       <c r="I12" s="177">
         <f t="shared" si="2"/>
-        <v>549427.02809841395</v>
+        <v>45785.58567486782</v>
       </c>
       <c r="J12" s="165"/>
     </row>
@@ -2087,11 +2097,11 @@
       </c>
       <c r="H15" s="16">
         <f t="shared" ref="H15:I15" si="4">SUM(H11:H14)</f>
-        <v>77094844.966881961</v>
+        <v>75695840.960149899</v>
       </c>
       <c r="I15" s="16">
         <f t="shared" si="4"/>
-        <v>27754144.188077506</v>
+        <v>27250502.745653957</v>
       </c>
       <c r="J15" s="170"/>
       <c r="K15" t="s">
@@ -2105,11 +2115,11 @@
     <row r="17" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="63"/>
       <c r="B17" s="64"/>
-      <c r="G17" s="185" t="s">
+      <c r="G17" s="184" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="185"/>
-      <c r="I17" s="185"/>
+      <c r="H17" s="184"/>
+      <c r="I17" s="184"/>
     </row>
     <row r="18" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="65"/>
@@ -2141,11 +2151,11 @@
       </c>
       <c r="H19" s="177">
         <f t="shared" si="6"/>
-        <v>7630930.9458113043</v>
+        <v>635910.91215094202</v>
       </c>
       <c r="I19" s="177">
         <f t="shared" si="6"/>
-        <v>2747135.1404920695</v>
+        <v>228927.9283743391</v>
       </c>
       <c r="J19" s="165"/>
     </row>
@@ -2199,11 +2209,11 @@
       </c>
       <c r="H22" s="16">
         <f t="shared" ref="H22" si="7">SUM(H18:H21)</f>
-        <v>385474224.83440983</v>
+        <v>378479204.80074942</v>
       </c>
       <c r="I22" s="16">
         <f t="shared" ref="I22" si="8">SUM(I18:I21)</f>
-        <v>138770720.94038752</v>
+        <v>136252513.72826979</v>
       </c>
       <c r="J22" s="170"/>
       <c r="L22"/>
@@ -2240,8 +2250,8 @@
         <v>2.6073019879409905E-3</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="188"/>
-      <c r="E25" s="188"/>
+      <c r="D25" s="187"/>
+      <c r="E25" s="187"/>
     </row>
     <row r="26" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="179" t="s">
@@ -2252,8 +2262,8 @@
         <v>3.1822804541266196E-3</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="188"/>
-      <c r="E26" s="188"/>
+      <c r="D26" s="187"/>
+      <c r="E26" s="187"/>
     </row>
     <row r="27" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="180" t="s">
@@ -2261,17 +2271,17 @@
       </c>
       <c r="B27" s="182">
         <f>'AWS web'!C19</f>
-        <v>0.15060466666666666</v>
-      </c>
-      <c r="C27" s="183">
+        <v>1.2550388888888889E-2</v>
+      </c>
+      <c r="C27" s="189">
         <f>B27*0.36</f>
-        <v>5.4217679999999997E-2</v>
-      </c>
-      <c r="D27" s="189">
+        <v>4.5181399999999995E-3</v>
+      </c>
+      <c r="D27" s="188">
         <f>C27/B26</f>
-        <v>17.037367001922558</v>
-      </c>
-      <c r="E27" s="189"/>
+        <v>1.4197805834935464</v>
+      </c>
+      <c r="E27" s="188"/>
     </row>
     <row r="28" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="180" t="s">
@@ -2281,15 +2291,15 @@
         <f>'AWS compute'!C17</f>
         <v>4.8583333333333339E-2</v>
       </c>
-      <c r="C28" s="183">
+      <c r="C28" s="189">
         <f t="shared" ref="C28:C30" si="9">B28*0.36</f>
         <v>1.7490000000000002E-2</v>
       </c>
-      <c r="D28" s="189">
+      <c r="D28" s="188">
         <f>C28/B26</f>
         <v>5.4960586447746484</v>
       </c>
-      <c r="E28" s="189"/>
+      <c r="E28" s="188"/>
     </row>
     <row r="29" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="180" t="s">
@@ -2299,15 +2309,15 @@
         <f>'AWS HM'!C17</f>
         <v>6.9987499999999994E-2</v>
       </c>
-      <c r="C29" s="183">
+      <c r="C29" s="189">
         <f t="shared" si="9"/>
         <v>2.5195499999999996E-2</v>
       </c>
-      <c r="D29" s="189">
+      <c r="D29" s="188">
         <f>C29/B26</f>
         <v>7.9174354250668735</v>
       </c>
-      <c r="E29" s="189"/>
+      <c r="E29" s="188"/>
       <c r="F29" s="178"/>
     </row>
     <row r="30" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2318,25 +2328,28 @@
         <f>'AWS GPU'!C17</f>
         <v>3.4319999999999999</v>
       </c>
-      <c r="C30" s="183">
+      <c r="C30" s="189">
         <f t="shared" si="9"/>
         <v>1.23552</v>
       </c>
-      <c r="D30" s="186">
-        <f>C30/(B26)*(30/10.6)</f>
-        <v>1098.820411144693</v>
-      </c>
-      <c r="E30" s="186"/>
-      <c r="F30" s="178"/>
+      <c r="D30" s="185">
+        <f>C30/((B26)*(30*128/10.6/2))</f>
+        <v>2.1434628714621122</v>
+      </c>
+      <c r="E30" s="185"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F31" s="174"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F32" s="174"/>
+      <c r="F32" s="178" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F33" s="174"/>
+      <c r="F33" s="190" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F34" s="175"/>
@@ -2362,7 +2375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419F1AD1-37B5-854B-8588-9C28ACDE4F4F}">
   <dimension ref="B1:N40"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -3052,7 +3065,7 @@
   <dimension ref="B3:K28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B19" sqref="B1:I19"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3330,8 +3343,8 @@
         <v>121</v>
       </c>
       <c r="I16" s="156">
-        <f>I15/C3</f>
-        <v>0.30120933333333333</v>
+        <f>I15/C3/12</f>
+        <v>2.5100777777777777E-2</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3346,7 +3359,7 @@
       </c>
       <c r="I17" s="106">
         <f>I16/2</f>
-        <v>0.15060466666666666</v>
+        <v>1.2550388888888889E-2</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>128</v>
@@ -3359,7 +3372,7 @@
       </c>
       <c r="C19" s="96">
         <f>I17</f>
-        <v>0.15060466666666666</v>
+        <v>1.2550388888888889E-2</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -4974,7 +4987,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="I17" s="184">
+      <c r="I17" s="183">
         <f>I14*0.36</f>
         <v>4.1349000000000004E-3</v>
       </c>

</xml_diff>